<commit_message>
working out gradient analysis
</commit_message>
<xml_diff>
--- a/analysis/thalamus/figures_tables/choroid_associations/hipsthomas_and_inflammatory_markers.xlsx
+++ b/analysis/thalamus/figures_tables/choroid_associations/hipsthomas_and_inflammatory_markers.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,431 +494,392 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>THALAMUS_1</t>
+          <t>AV_2</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-0.4233475868868328</v>
+        <v>0.03556268867412338</v>
       </c>
       <c r="D2" t="n">
-        <v>3.496055685379108e-24</v>
+        <v>0.3376318019411778</v>
       </c>
       <c r="E2" t="n">
-        <v>0.04654206149278174</v>
+        <v>0.04119571369779234</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.5007941824296606</v>
+        <v>-0.03724506997980553</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.3459009913440051</v>
+        <v>0.1083704473280523</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>[-0.500794, -0.345901]</t>
+          <t>[-0.037245, 0.108370]</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>1.281887084639006e-23</v>
+        <v>0.3376318019411778</v>
       </c>
       <c r="J2" t="n">
-        <v>0.4305582158086486</v>
+        <v>0.5615757194326364</v>
       </c>
       <c r="K2" t="n">
-        <v>-0.4233475868868328</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>AV_2</t>
+          <t>VA_4</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>-0.2550761262983671</v>
+        <v>0.179249731107587</v>
       </c>
       <c r="D3" t="n">
-        <v>4.860703906741938e-09</v>
+        <v>1.321608312741613e-07</v>
       </c>
       <c r="E3" t="n">
-        <v>0.04531946610693682</v>
+        <v>0.02937651815853129</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.3391068764261562</v>
+        <v>0.1135232392020837</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.171045376170578</v>
+        <v>0.2449762230130904</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>[-0.339107, -0.171045]</t>
+          <t>[0.113523, 0.244976]</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>5.94086033046237e-09</v>
+        <v>1.321608312741613e-06</v>
       </c>
       <c r="J3" t="n">
-        <v>0.2704439230077779</v>
+        <v>0.6747961542970171</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.2550761262983671</v>
+        <v>0.179249731107587</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>VA_4</t>
+          <t>VLa_5</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-0.1034018233359098</v>
+        <v>0.1407527676120614</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0097181972288605</v>
+        <v>0.0001350786416931663</v>
       </c>
       <c r="E4" t="n">
-        <v>0.04190800766410111</v>
+        <v>0.03699986415169781</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.1816599732808754</v>
+        <v>0.06889894463193036</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.02514367339094419</v>
+        <v>0.2126065905921924</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>[-0.181660, -0.025144]</t>
+          <t>[0.068899, 0.212607]</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>0.0097181972288605</v>
+        <v>0.0004502621389772209</v>
       </c>
       <c r="J4" t="n">
-        <v>0.4240605270197837</v>
+        <v>0.5871373976814684</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.1034018233359098</v>
+        <v>0.1407527676120614</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>VLa_5</t>
+          <t>VLP_6</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>-0.1087260684390325</v>
+        <v>0.1122815941100022</v>
       </c>
       <c r="D5" t="n">
-        <v>0.006938025145978363</v>
+        <v>7.848105010194994e-06</v>
       </c>
       <c r="E5" t="n">
-        <v>0.04098864795208087</v>
+        <v>0.02414391858429712</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.1875101882984618</v>
+        <v>0.06347175554489978</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.02994194857960321</v>
+        <v>0.1610914326751046</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>[-0.187510, -0.029942]</t>
+          <t>[0.063472, 0.161091]</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>0.0076318276605762</v>
+        <v>3.924052505097497e-05</v>
       </c>
       <c r="J5" t="n">
-        <v>0.3799508942401152</v>
+        <v>0.8170643622529261</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.1087260684390325</v>
+        <v>0.1122815941100022</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>VLP_6</t>
+          <t>VPL_7</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>-0.261330845021461</v>
+        <v>0.08821922703435416</v>
       </c>
       <c r="D6" t="n">
-        <v>5.678227701686726e-10</v>
+        <v>0.002359569946564645</v>
       </c>
       <c r="E6" t="n">
-        <v>0.04957941742833478</v>
+        <v>0.02766769595802581</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.342413760698728</v>
+        <v>0.03152350230200214</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.180247929344194</v>
+        <v>0.1449149517667062</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>[-0.342414, -0.180248]</t>
+          <t>[0.031524, 0.144915]</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>7.807563089819248e-10</v>
+        <v>0.004719139893129289</v>
       </c>
       <c r="J6" t="n">
-        <v>0.369354625686202</v>
+        <v>0.7516061408634798</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.261330845021461</v>
+        <v>0.08821922703435416</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>VPL_7</t>
+          <t>Pul_8</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-0.2833562070267958</v>
+        <v>-0.04004361872010605</v>
       </c>
       <c r="D7" t="n">
-        <v>1.376503653801543e-10</v>
+        <v>0.03383510450411615</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0490458222259991</v>
+        <v>0.01800900038457809</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.3681395400258516</v>
+        <v>-0.07701568854194923</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.19857287402774</v>
+        <v>-0.00307154889826286</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>[-0.368140, -0.198573]</t>
+          <t>[-0.077016, -0.003072]</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>2.163077170259567e-10</v>
+        <v>0.04229388063014519</v>
       </c>
       <c r="J7" t="n">
-        <v>0.3060884319495186</v>
+        <v>0.8943056963311456</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.2833562070267958</v>
+        <v>-0.04004361872010605</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Pul_8</t>
+          <t>LGN_9</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>-0.4494165277926355</v>
+        <v>-0.07310772784412721</v>
       </c>
       <c r="D8" t="n">
-        <v>2.320345642984334e-24</v>
+        <v>0.05723033469196295</v>
       </c>
       <c r="E8" t="n">
-        <v>0.04620181185443084</v>
+        <v>0.04147888925412969</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.531272388139773</v>
+        <v>-0.1484705800025682</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.367560667445498</v>
+        <v>0.002255124314313836</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>[-0.531272, -0.367561]</t>
+          <t>[-0.148471, 0.002255]</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>1.276190103641384e-23</v>
+        <v>0.06358926076884773</v>
       </c>
       <c r="J8" t="n">
-        <v>0.3527880433595429</v>
+        <v>0.5587967123142135</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.4494165277926355</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>LGN_9</t>
+          <t>MGN_10</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>-0.3910357195779562</v>
+        <v>-0.07323478832335117</v>
       </c>
       <c r="D9" t="n">
-        <v>9.554374061842789e-17</v>
+        <v>0.02034436255117691</v>
       </c>
       <c r="E9" t="n">
-        <v>0.04919619906563672</v>
+        <v>0.03039346454512853</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.4800264975691568</v>
+        <v>-0.1350544471193587</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.3020449415867557</v>
+        <v>-0.0114151295273437</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>[-0.480026, -0.302045]</t>
+          <t>[-0.135054, -0.011415]</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>1.751635244671178e-16</v>
+        <v>0.02906337507310988</v>
       </c>
       <c r="J9" t="n">
-        <v>0.2314767360540894</v>
+        <v>0.7058416598547887</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.3910357195779562</v>
+        <v>-0.07323478832335117</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>MGN_10</t>
+          <t>CM_11</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>-0.3795620589117831</v>
+        <v>-0.1024871769788244</v>
       </c>
       <c r="D10" t="n">
-        <v>1.349999452217697e-19</v>
+        <v>0.003888489664059669</v>
       </c>
       <c r="E10" t="n">
-        <v>0.04027819138774348</v>
+        <v>0.03755330347488479</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.4582575909558014</v>
+        <v>-0.1718938343686608</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.3008665268677648</v>
+        <v>-0.03308051958898803</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>[-0.458258, -0.300867]</t>
+          <t>[-0.171894, -0.033081]</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>3.712498493598665e-19</v>
+        <v>0.006480816106766115</v>
       </c>
       <c r="J10" t="n">
-        <v>0.4045147143283261</v>
+        <v>0.6224402017305293</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.3795620589117831</v>
+        <v>-0.1024871769788244</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>CM_11</t>
+          <t>MD_Pf_12</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>-0.3685287059393024</v>
+        <v>-0.06911014778523375</v>
       </c>
       <c r="D11" t="n">
-        <v>1.383168420836368e-18</v>
+        <v>0.001179599562757957</v>
       </c>
       <c r="E11" t="n">
-        <v>0.04184330124271129</v>
+        <v>0.0213192233561758</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.4473739056926054</v>
+        <v>-0.1107169855519313</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.2896835061859995</v>
+        <v>-0.02750331001853618</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>[-0.447374, -0.289684]</t>
+          <t>[-0.110717, -0.027503]</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>3.04297052584001e-18</v>
+        <v>0.002948998906894892</v>
       </c>
       <c r="J11" t="n">
-        <v>0.391336966424178</v>
+        <v>0.8719435675628403</v>
       </c>
       <c r="K11" t="n">
-        <v>-0.3685287059393024</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>MD_Pf_12</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>-0.4674396944775042</v>
-      </c>
-      <c r="D12" t="n">
-        <v>4.881371335465726e-26</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.04661822375944124</v>
-      </c>
-      <c r="F12" t="n">
-        <v>-0.5492490733518977</v>
-      </c>
-      <c r="G12" t="n">
-        <v>-0.3856303156031107</v>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>[-0.549249, -0.385630]</t>
-        </is>
-      </c>
-      <c r="I12" t="n">
-        <v>5.369508469012299e-25</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0.3815265024246141</v>
-      </c>
-      <c r="K12" t="n">
-        <v>-0.4674396944775042</v>
+        <v>-0.06911014778523375</v>
       </c>
     </row>
   </sheetData>
@@ -932,7 +893,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -994,431 +955,392 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>THALAMUS_1</t>
+          <t>AV_2</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-0.5673222863704793</v>
+        <v>0.06604805841085898</v>
       </c>
       <c r="D2" t="n">
-        <v>1.7316828664463e-47</v>
+        <v>0.109488457680669</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0440324656567952</v>
+        <v>0.04721212671916925</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.6357453107355809</v>
+        <v>-0.01489049544206832</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.4988992620053777</v>
+        <v>0.1469866122637863</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>[-0.635745, -0.498899]</t>
+          <t>[-0.014890, 0.146987]</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>9.524255765454651e-47</v>
+        <v>0.12165384186741</v>
       </c>
       <c r="J2" t="n">
-        <v>0.5481477709958016</v>
+        <v>0.562530608952704</v>
       </c>
       <c r="K2" t="n">
-        <v>-0.5673222863704793</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>AV_2</t>
+          <t>VA_4</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>-0.3379841006158725</v>
+        <v>0.1875569997159206</v>
       </c>
       <c r="D3" t="n">
-        <v>2.046508920914253e-15</v>
+        <v>5.610344642785792e-07</v>
       </c>
       <c r="E3" t="n">
-        <v>0.04084958644046719</v>
+        <v>0.03565247771474309</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.4187668212414911</v>
+        <v>0.1149421012820964</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.257201379990254</v>
+        <v>0.2601718981497448</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>[-0.418767, -0.257201]</t>
+          <t>[0.114942, 0.260172]</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>2.50128868111742e-15</v>
+        <v>1.870114880928597e-06</v>
       </c>
       <c r="J3" t="n">
-        <v>0.3137900163602401</v>
+        <v>0.6777290787900128</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.3379841006158725</v>
+        <v>0.1875569997159206</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>VA_4</t>
+          <t>VLa_5</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-0.2124223020686351</v>
+        <v>0.120398186682097</v>
       </c>
       <c r="D4" t="n">
-        <v>4.969533502517732e-08</v>
+        <v>0.003424485496804276</v>
       </c>
       <c r="E4" t="n">
-        <v>0.03971293843308061</v>
+        <v>0.04445421673701932</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.2877118470609478</v>
+        <v>0.03997969004779968</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.1371327570763223</v>
+        <v>0.2008166833163944</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>[-0.287712, -0.137133]</t>
+          <t>[0.039980, 0.200817]</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>4.969533502517732e-08</v>
+        <v>0.005707475828007127</v>
       </c>
       <c r="J4" t="n">
-        <v>0.4544654157897234</v>
+        <v>0.5824235860046931</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.2124223020686351</v>
+        <v>0.120398186682097</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>VLa_5</t>
+          <t>VLP_6</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>-0.2205094989624254</v>
+        <v>0.1312091981979246</v>
       </c>
       <c r="D5" t="n">
-        <v>2.192700385996757e-08</v>
+        <v>2.619087690934368e-06</v>
       </c>
       <c r="E5" t="n">
-        <v>0.04426013459457132</v>
+        <v>0.03691941172766573</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.2965927422924334</v>
+        <v>0.07701884184008226</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.1444262556324175</v>
+        <v>0.185399554555767</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>[-0.296593, -0.144426]</t>
+          <t>[0.077019, 0.185400]</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>2.411970424596432e-08</v>
+        <v>6.547719227335919e-06</v>
       </c>
       <c r="J5" t="n">
-        <v>0.4114472588889586</v>
+        <v>0.8181709271365641</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.2205094989624254</v>
+        <v>0.1312091981979246</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>VLP_6</t>
+          <t>VPL_7</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>-0.3874626266628118</v>
+        <v>0.1612379887265692</v>
       </c>
       <c r="D6" t="n">
-        <v>1.623262121907625e-21</v>
+        <v>4.762324244893822e-07</v>
       </c>
       <c r="E6" t="n">
-        <v>0.04865527555887444</v>
+        <v>0.03534496105305199</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.4634499189518968</v>
+        <v>0.09921378685864968</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.3114753343737269</v>
+        <v>0.2232621905944887</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>[-0.463450, -0.311475]</t>
+          <t>[0.099214, 0.223262]</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>2.55084047728341e-21</v>
+        <v>1.870114880928597e-06</v>
       </c>
       <c r="J6" t="n">
-        <v>0.4370309238106785</v>
+        <v>0.7602809142358191</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.3874626266628118</v>
+        <v>0.1612379887265692</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>VPL_7</t>
+          <t>Pul_8</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-0.3718574937566554</v>
+        <v>-0.0154282494445978</v>
       </c>
       <c r="D7" t="n">
-        <v>5.285885300373449e-18</v>
+        <v>0.4591550883972508</v>
       </c>
       <c r="E7" t="n">
-        <v>0.05041138271154486</v>
+        <v>0.02421515327230556</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.4529232141990606</v>
+        <v>-0.05635147660402158</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.2907917733142503</v>
+        <v>0.02549497771482597</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>[-0.452923, -0.290792]</t>
+          <t>[-0.056351, 0.025495]</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>7.268092288013492e-18</v>
+        <v>0.4591550883972508</v>
       </c>
       <c r="J7" t="n">
-        <v>0.3551806995455838</v>
+        <v>0.895067750242079</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.3718574937566554</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Pul_8</t>
+          <t>LGN_9</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>-0.5687358149461191</v>
+        <v>-0.1280625921041529</v>
       </c>
       <c r="D8" t="n">
-        <v>6.078402581144763e-42</v>
+        <v>0.002688599817434789</v>
       </c>
       <c r="E8" t="n">
-        <v>0.04593471815971089</v>
+        <v>0.0544463254121262</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.6429955246462746</v>
+        <v>-0.2114586092113173</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.4944761052459636</v>
+        <v>-0.04466657499698863</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>[-0.642996, -0.494476]</t>
+          <t>[-0.211459, -0.044667]</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>2.228747613086413e-41</v>
+        <v>0.005377199634869577</v>
       </c>
       <c r="J8" t="n">
-        <v>0.4559246868369051</v>
+        <v>0.5643907012606564</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.5687358149461191</v>
+        <v>-0.1280625921041529</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>LGN_9</t>
+          <t>MGN_10</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>-0.5270941502223708</v>
+        <v>-0.07045745999058152</v>
       </c>
       <c r="D9" t="n">
-        <v>1.250916715400871e-31</v>
+        <v>0.0451668331116468</v>
       </c>
       <c r="E9" t="n">
-        <v>0.04979540970280934</v>
+        <v>0.03462947594240112</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.6090901654525204</v>
+        <v>-0.1393913282000977</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.4450981349922213</v>
+        <v>-0.001523591781065356</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>[-0.609090, -0.445098]</t>
+          <t>[-0.139391, -0.001524]</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>2.752016773881916e-31</v>
+        <v>0.0564585413895585</v>
       </c>
       <c r="J9" t="n">
-        <v>0.3369056795242069</v>
+        <v>0.7050913300657735</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.5270941502223708</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>MGN_10</t>
+          <t>CM_11</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>-0.4749221523114865</v>
+        <v>-0.09986839484596156</v>
       </c>
       <c r="D10" t="n">
-        <v>5.937320485414924e-32</v>
+        <v>0.01146222464445488</v>
       </c>
       <c r="E10" t="n">
-        <v>0.04091655714345117</v>
+        <v>0.03828633168576921</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.5483443628198725</v>
+        <v>-0.1771806330516393</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.4014999418031005</v>
+        <v>-0.02255615664028383</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>[-0.548344, -0.401500]</t>
+          <t>[-0.177181, -0.022556]</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>1.632763133489104e-31</v>
+        <v>0.01637460663493555</v>
       </c>
       <c r="J10" t="n">
-        <v>0.4731821962658569</v>
+        <v>0.6218047102593067</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.4749221523114865</v>
+        <v>-0.09986839484596156</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>CM_11</t>
+          <t>MD_Pf_12</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>-0.4476354640356413</v>
+        <v>-0.1335389969087319</v>
       </c>
       <c r="D11" t="n">
-        <v>2.585654574876497e-28</v>
+        <v>1.233579902195876e-08</v>
       </c>
       <c r="E11" t="n">
-        <v>0.04214550557682581</v>
+        <v>0.0265437856068387</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.5221129548507999</v>
+        <v>-0.178784648307407</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.3731579732204827</v>
+        <v>-0.08829334551005681</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>[-0.522113, -0.373158]</t>
+          <t>[-0.178785, -0.088293]</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>4.74036672060691e-28</v>
+        <v>1.233579902195876e-07</v>
       </c>
       <c r="J11" t="n">
-        <v>0.4473464208619148</v>
+        <v>0.877806720999931</v>
       </c>
       <c r="K11" t="n">
-        <v>-0.4476354640356413</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>MD_Pf_12</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>-0.6370546949377049</v>
-      </c>
-      <c r="D12" t="n">
-        <v>4.892085501271023e-54</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.04785143012215663</v>
-      </c>
-      <c r="F12" t="n">
-        <v>-0.7076599127078019</v>
-      </c>
-      <c r="G12" t="n">
-        <v>-0.566449477167608</v>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>[-0.707660, -0.566449]</t>
-        </is>
-      </c>
-      <c r="I12" t="n">
-        <v>5.381294051398125e-53</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0.5314558568871625</v>
-      </c>
-      <c r="K12" t="n">
-        <v>-0.6370546949377049</v>
+        <v>-0.1335389969087319</v>
       </c>
     </row>
   </sheetData>
@@ -1432,7 +1354,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1494,431 +1416,392 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>THALAMUS_1</t>
+          <t>AV_2</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.6032557794611566</v>
+        <v>0.04135601069455529</v>
       </c>
       <c r="D2" t="n">
-        <v>1.365852612777161e-51</v>
+        <v>0.3396210627434858</v>
       </c>
       <c r="E2" t="n">
-        <v>0.04666693064312565</v>
+        <v>0.04644110668331872</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5343020677969886</v>
+        <v>-0.04366221673281095</v>
       </c>
       <c r="G2" t="n">
-        <v>0.6722094911253246</v>
+        <v>0.1263742381219215</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>[0.534302, 0.672209]</t>
+          <t>[-0.043662, 0.126374]</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>1.502437874054878e-50</v>
+        <v>0.4387494008791866</v>
       </c>
       <c r="J2" t="n">
-        <v>0.5658160025990456</v>
+        <v>0.561568554808358</v>
       </c>
       <c r="K2" t="n">
-        <v>0.6032557794611566</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>AV_2</t>
+          <t>VA_4</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.4292826919464522</v>
+        <v>-0.09009688328699142</v>
       </c>
       <c r="D3" t="n">
-        <v>1.527592071219643e-23</v>
+        <v>0.02488087746746357</v>
       </c>
       <c r="E3" t="n">
-        <v>0.04298617539079432</v>
+        <v>0.03743556678941224</v>
       </c>
       <c r="F3" t="n">
-        <v>0.3494810914704206</v>
+        <v>-0.1687652616702969</v>
       </c>
       <c r="G3" t="n">
-        <v>0.5090842924224839</v>
+        <v>-0.0114285049036859</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>[0.349481, 0.509084]</t>
+          <t>[-0.168765, -0.011429]</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>2.100439097927009e-23</v>
+        <v>0.1244043873373178</v>
       </c>
       <c r="J3" t="n">
-        <v>0.3671230933326022</v>
+        <v>0.6583247729242681</v>
       </c>
       <c r="K3" t="n">
-        <v>0.4292826919464522</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>VA_4</t>
+          <t>VLa_5</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.2968202594815147</v>
+        <v>-0.07098386611194066</v>
       </c>
       <c r="D4" t="n">
-        <v>7.819613078906771e-14</v>
+        <v>0.1014271795289936</v>
       </c>
       <c r="E4" t="n">
-        <v>0.04036513345293061</v>
+        <v>0.04144925638887547</v>
       </c>
       <c r="F4" t="n">
-        <v>0.2211561790804741</v>
+        <v>-0.1559750029525444</v>
       </c>
       <c r="G4" t="n">
-        <v>0.3724843398825554</v>
+        <v>0.01400727072866305</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>[0.221156, 0.372484]</t>
+          <t>[-0.155975, 0.014007]</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>8.601574386797449e-14</v>
+        <v>0.2028543590579872</v>
       </c>
       <c r="J4" t="n">
-        <v>0.4821415648375091</v>
+        <v>0.5763654311030935</v>
       </c>
       <c r="K4" t="n">
-        <v>0.2968202594815147</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>VLa_5</t>
+          <t>VLP_6</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.2721599813497476</v>
+        <v>-0.04407187142001324</v>
       </c>
       <c r="D5" t="n">
-        <v>1.324127341163287e-11</v>
+        <v>0.1367554383463904</v>
       </c>
       <c r="E5" t="n">
-        <v>0.04605900154076487</v>
+        <v>0.02659012928132522</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1951032023832701</v>
+        <v>-0.1021743807048659</v>
       </c>
       <c r="G5" t="n">
-        <v>0.3492167603162252</v>
+        <v>0.01403063786483939</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>[0.195103, 0.349217]</t>
+          <t>[-0.102174, 0.014031]</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>1.324127341163287e-11</v>
+        <v>0.2279257305773173</v>
       </c>
       <c r="J5" t="n">
-        <v>0.4294624144391187</v>
+        <v>0.8098870581079389</v>
       </c>
       <c r="K5" t="n">
-        <v>0.2721599813497476</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>VLP_6</t>
+          <t>VPL_7</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.4735658795833201</v>
+        <v>-0.05886365628701076</v>
       </c>
       <c r="D6" t="n">
-        <v>4.963074253302894e-31</v>
+        <v>0.08332676005318713</v>
       </c>
       <c r="E6" t="n">
-        <v>0.04882275661510523</v>
+        <v>0.03699150338096954</v>
       </c>
       <c r="F6" t="n">
-        <v>0.3990218081438131</v>
+        <v>-0.1255168250678584</v>
       </c>
       <c r="G6" t="n">
-        <v>0.5481099510228271</v>
+        <v>0.007789512493836928</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>[0.399022, 0.548110]</t>
+          <t>[-0.125517, 0.007790]</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>1.364845419658296e-30</v>
+        <v>0.2028543590579872</v>
       </c>
       <c r="J6" t="n">
-        <v>0.4872961648035454</v>
+        <v>0.7482206178421502</v>
       </c>
       <c r="K6" t="n">
-        <v>0.4735658795833201</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>VPL_7</t>
+          <t>Pul_8</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.4684753179772765</v>
+        <v>0.01435764133640541</v>
       </c>
       <c r="D7" t="n">
-        <v>2.428422819882067e-27</v>
+        <v>0.515597352908955</v>
       </c>
       <c r="E7" t="n">
-        <v>0.04816881475702234</v>
+        <v>0.02417699578528845</v>
       </c>
       <c r="F7" t="n">
-        <v>0.3888577881901966</v>
+        <v>-0.0290058750508658</v>
       </c>
       <c r="G7" t="n">
-        <v>0.5480928477643563</v>
+        <v>0.05772115772367661</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>[0.388858, 0.548093]</t>
+          <t>[-0.029006, 0.057721]</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>3.81609300267182e-27</v>
+        <v>0.5728859476766167</v>
       </c>
       <c r="J7" t="n">
-        <v>0.4114079364579352</v>
+        <v>0.893367064263339</v>
       </c>
       <c r="K7" t="n">
-        <v>0.4684753179772765</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Pul_8</t>
+          <t>LGN_9</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.6034892376006605</v>
+        <v>0.08800578168279302</v>
       </c>
       <c r="D8" t="n">
-        <v>5.307523417322506e-45</v>
+        <v>0.04993159816293799</v>
       </c>
       <c r="E8" t="n">
-        <v>0.04241281502122524</v>
+        <v>0.05212827785741764</v>
       </c>
       <c r="F8" t="n">
-        <v>0.5281247527428271</v>
+        <v>2.639238674287392e-05</v>
       </c>
       <c r="G8" t="n">
-        <v>0.678853722458494</v>
+        <v>0.1759851709788432</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>[0.528125, 0.678854]</t>
+          <t>[0.000026, 0.175985]</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>1.946091919684919e-44</v>
+        <v>0.1664386605431266</v>
       </c>
       <c r="J8" t="n">
-        <v>0.4722912516300214</v>
+        <v>0.5590145077226707</v>
       </c>
       <c r="K8" t="n">
-        <v>0.6034892376006605</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>LGN_9</t>
+          <t>MGN_10</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.5275347203488316</v>
+        <v>0.01930889284069786</v>
       </c>
       <c r="D9" t="n">
-        <v>8.114358000783039e-30</v>
+        <v>0.6014078764523675</v>
       </c>
       <c r="E9" t="n">
-        <v>0.04291406481128502</v>
+        <v>0.03789461928095734</v>
       </c>
       <c r="F9" t="n">
-        <v>0.4424574081227824</v>
+        <v>-0.05327854249468314</v>
       </c>
       <c r="G9" t="n">
-        <v>0.6126120325748808</v>
+        <v>0.09189632817607885</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>[0.442457, 0.612612]</t>
+          <t>[-0.053279, 0.091896]</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>1.785158760172269e-29</v>
+        <v>0.6014078764523675</v>
       </c>
       <c r="J9" t="n">
-        <v>0.3243708467257745</v>
+        <v>0.7025669724722581</v>
       </c>
       <c r="K9" t="n">
-        <v>0.5275347203488316</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>MGN_10</t>
+          <t>CM_11</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.4691103378893504</v>
+        <v>-0.03881652701647562</v>
       </c>
       <c r="D10" t="n">
-        <v>2.823999872684555e-29</v>
+        <v>0.3509995207033493</v>
       </c>
       <c r="E10" t="n">
-        <v>0.04534624468101713</v>
+        <v>0.0402672056776747</v>
       </c>
       <c r="F10" t="n">
-        <v>0.3926099169657057</v>
+        <v>-0.1205207640640961</v>
       </c>
       <c r="G10" t="n">
-        <v>0.5456107588129951</v>
+        <v>0.04288771003114488</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>[0.392610, 0.545611]</t>
+          <t>[-0.120521, 0.042888]</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>5.177333099921683e-29</v>
+        <v>0.4387494008791866</v>
       </c>
       <c r="J10" t="n">
-        <v>0.4587319658073303</v>
+        <v>0.6162830594768768</v>
       </c>
       <c r="K10" t="n">
-        <v>0.4691103378893504</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>CM_11</t>
+          <t>MD_Pf_12</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.3845429101963909</v>
+        <v>0.06924677880854328</v>
       </c>
       <c r="D11" t="n">
-        <v>1.825109276836998e-19</v>
+        <v>0.005449229458446015</v>
       </c>
       <c r="E11" t="n">
-        <v>0.04667010569488469</v>
+        <v>0.02958131242993796</v>
       </c>
       <c r="F11" t="n">
-        <v>0.3044969010268013</v>
+        <v>0.02051501916836029</v>
       </c>
       <c r="G11" t="n">
-        <v>0.4645889193659805</v>
+        <v>0.1179785384487263</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>[0.304497, 0.464589]</t>
+          <t>[0.020515, 0.117979]</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>2.230689116134109e-19</v>
+        <v>0.05449229458446016</v>
       </c>
       <c r="J11" t="n">
-        <v>0.3965801028420753</v>
+        <v>0.8711648121262665</v>
       </c>
       <c r="K11" t="n">
-        <v>0.3845429101963909</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>MD_Pf_12</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>0.6295179925606446</v>
-      </c>
-      <c r="D12" t="n">
-        <v>6.183327826629986e-49</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.05004220057883693</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.5550363924930409</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0.7039995926282482</v>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>[0.555036, 0.704000]</t>
-        </is>
-      </c>
-      <c r="I12" t="n">
-        <v>3.400830304646492e-48</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0.5069093737091628</v>
-      </c>
-      <c r="K12" t="n">
-        <v>0.6295179925606446</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1932,7 +1815,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1994,431 +1877,392 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>THALAMUS_1</t>
+          <t>AV_2</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-0.3610932528872888</v>
+        <v>-0.0330401528532079</v>
       </c>
       <c r="D2" t="n">
-        <v>1.763671834582291e-21</v>
+        <v>0.3175529057590162</v>
       </c>
       <c r="E2" t="n">
-        <v>0.08139067231182584</v>
+        <v>0.03025233076423178</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.4319871913468228</v>
+        <v>-0.09793001571014844</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.2901993144277548</v>
+        <v>0.03184971000373264</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>[-0.431987, -0.290199]</t>
+          <t>[-0.097930, 0.031850]</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>9.700195090202601e-21</v>
+        <v>0.3528365619544625</v>
       </c>
       <c r="J2" t="n">
-        <v>0.4151837151356217</v>
+        <v>0.561651328766432</v>
       </c>
       <c r="K2" t="n">
-        <v>-0.3610932528872888</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>AV_2</t>
+          <t>VA_4</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>-0.2690110020718494</v>
+        <v>0.06839737723192107</v>
       </c>
       <c r="D3" t="n">
-        <v>5.976030309491399e-12</v>
+        <v>0.02568504118677124</v>
       </c>
       <c r="E3" t="n">
-        <v>0.06473177318843247</v>
+        <v>0.04793439989100107</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.3438473836785813</v>
+        <v>0.008344763286117357</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.1941746204651175</v>
+        <v>0.1284499911777248</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>[-0.343847, -0.194175]</t>
+          <t>[0.008345, 0.128450]</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>9.390904772057913e-12</v>
+        <v>0.05137008237354248</v>
       </c>
       <c r="J3" t="n">
-        <v>0.2908071614</v>
+        <v>0.6582840060735957</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.2690110020718494</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>VA_4</t>
+          <t>VLa_5</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-0.154354987991408</v>
+        <v>0.0755101050291163</v>
       </c>
       <c r="D4" t="n">
-        <v>1.704936981641276e-05</v>
+        <v>0.02226423207573674</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0397679437635684</v>
+        <v>0.04347532667441587</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.2241472984771726</v>
+        <v>0.01081322320908462</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.0845626775056434</v>
+        <v>0.140206986849148</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>[-0.224147, -0.084563]</t>
+          <t>[0.010813, 0.140207]</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>1.875430679805404e-05</v>
+        <v>0.05137008237354248</v>
       </c>
       <c r="J4" t="n">
-        <v>0.4385780036127892</v>
+        <v>0.5786924977222758</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.154354987991408</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>VLa_5</t>
+          <t>VLP_6</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>-0.1267636467417341</v>
+        <v>0.06393005544567905</v>
       </c>
       <c r="D5" t="n">
-        <v>0.00047584603813525</v>
+        <v>0.004558975170413219</v>
       </c>
       <c r="E5" t="n">
-        <v>0.04148139846369063</v>
+        <v>0.03331015935387158</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.1975502161922583</v>
+        <v>0.01985870300508957</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.05597707729120981</v>
+        <v>0.1080014078862685</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>[-0.197550, -0.055977]</t>
+          <t>[0.019859, 0.108001]</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>0.00047584603813525</v>
+        <v>0.04558975170413219</v>
       </c>
       <c r="J5" t="n">
-        <v>0.3865106577308808</v>
+        <v>0.8122745993720693</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.1267636467417341</v>
+        <v>0.06393005544567905</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>VLP_6</t>
+          <t>VPL_7</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>-0.2470079231184585</v>
+        <v>0.01308783596852469</v>
       </c>
       <c r="D6" t="n">
-        <v>8.033007590474896e-11</v>
+        <v>0.6144964412878282</v>
       </c>
       <c r="E6" t="n">
-        <v>0.05948879944485699</v>
+        <v>0.02341533446270788</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.3199464895263614</v>
+        <v>-0.03794130448554402</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.1740693567105557</v>
+        <v>0.0641169764225934</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>[-0.319946, -0.174069]</t>
+          <t>[-0.037941, 0.064117]</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>1.104538543690298e-10</v>
+        <v>0.6144964412878282</v>
       </c>
       <c r="J6" t="n">
-        <v>0.3745428989154543</v>
+        <v>0.7467185137609449</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.2470079231184585</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>VPL_7</t>
+          <t>Pul_8</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-0.2911630732619155</v>
+        <v>-0.03805094281859603</v>
       </c>
       <c r="D7" t="n">
-        <v>1.959357327287349e-13</v>
+        <v>0.02363313653326579</v>
       </c>
       <c r="E7" t="n">
-        <v>0.06463849276564204</v>
+        <v>0.02105954243609407</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.3666896669437795</v>
+        <v>-0.07098304600584844</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.2156364795800514</v>
+        <v>-0.005118839631343616</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>[-0.366690, -0.215636]</t>
+          <t>[-0.070983, -0.005119]</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>3.592155100026807e-13</v>
+        <v>0.05137008237354248</v>
       </c>
       <c r="J7" t="n">
-        <v>0.32509983574791</v>
+        <v>0.8944472153367604</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.2911630732619155</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Pul_8</t>
+          <t>LGN_9</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>-0.3872697068736399</v>
+        <v>-0.07925793541513584</v>
       </c>
       <c r="D8" t="n">
-        <v>4.293796143896245e-22</v>
+        <v>0.02061042022673765</v>
       </c>
       <c r="E8" t="n">
-        <v>0.08786133959017055</v>
+        <v>0.04607743442705105</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.4620393322417358</v>
+        <v>-0.1463040459459171</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.3125000815055439</v>
+        <v>-0.01221182488435463</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>[-0.462039, -0.312500]</t>
+          <t>[-0.146304, -0.012212]</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>4.72317575828587e-21</v>
+        <v>0.05137008237354248</v>
       </c>
       <c r="J8" t="n">
-        <v>0.338158543167472</v>
+        <v>0.5604604368949375</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.3872697068736399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>LGN_9</t>
+          <t>MGN_10</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>-0.3487751022128497</v>
+        <v>-0.0546634553384805</v>
       </c>
       <c r="D9" t="n">
-        <v>2.449768556868147e-16</v>
+        <v>0.05225060610286177</v>
       </c>
       <c r="E9" t="n">
-        <v>0.08826489511453021</v>
+        <v>0.02280834173416717</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.4293200681224424</v>
+        <v>-0.1098613930005997</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.2682301363032569</v>
+        <v>0.0005344823236387297</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>[-0.429320, -0.268230]</t>
+          <t>[-0.109861, 0.000534]</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>5.389490825109923e-16</v>
+        <v>0.08708434350476961</v>
       </c>
       <c r="J9" t="n">
-        <v>0.2283854706710828</v>
+        <v>0.7048108642573608</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.3487751022128497</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>MGN_10</t>
+          <t>CM_11</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>-0.3186824469609734</v>
+        <v>0.05611989581515185</v>
       </c>
       <c r="D10" t="n">
-        <v>6.025835487667558e-17</v>
+        <v>0.0769500920124073</v>
       </c>
       <c r="E10" t="n">
-        <v>0.06560748342673889</v>
+        <v>0.03211467865491727</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.3906982691641652</v>
+        <v>-0.00609405633533662</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.2466666247577816</v>
+        <v>0.1183338479656403</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>[-0.390698, -0.246667]</t>
+          <t>[-0.006094, 0.118334]</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>1.657104759108578e-16</v>
+        <v>0.1099287028748676</v>
       </c>
       <c r="J10" t="n">
-        <v>0.3888000489323051</v>
+        <v>0.6181561716162576</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.3186824469609734</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>CM_11</t>
+          <t>MD_Pf_12</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>-0.1982219078520405</v>
+        <v>-0.02886133717329353</v>
       </c>
       <c r="D11" t="n">
-        <v>3.425855628508929e-07</v>
+        <v>0.1302654335430481</v>
       </c>
       <c r="E11" t="n">
-        <v>0.06976463669598602</v>
+        <v>0.01723500754408516</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.273512535075437</v>
+        <v>-0.06627885974334326</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.122931280628644</v>
+        <v>0.008556185396756191</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>[-0.273513, -0.122931]</t>
+          <t>[-0.066279, 0.008556]</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>4.187156879288691e-07</v>
+        <v>0.1628317919288102</v>
       </c>
       <c r="J11" t="n">
-        <v>0.3197558398477046</v>
+        <v>0.8696386811636705</v>
       </c>
       <c r="K11" t="n">
-        <v>-0.1982219078520405</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>MD_Pf_12</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>-0.3752414118270813</v>
-      </c>
-      <c r="D12" t="n">
-        <v>2.157618247814793e-20</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.08520338130647116</v>
-      </c>
-      <c r="F12" t="n">
-        <v>-0.4512232336147959</v>
-      </c>
-      <c r="G12" t="n">
-        <v>-0.2992595900393666</v>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>[-0.451223, -0.299260]</t>
-        </is>
-      </c>
-      <c r="I12" t="n">
-        <v>7.911266908654242e-20</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0.3461307871639431</v>
-      </c>
-      <c r="K12" t="n">
-        <v>-0.3752414118270813</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2432,7 +2276,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2494,431 +2338,392 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>THALAMUS_1</t>
+          <t>AV_2</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-0.2828481460571259</v>
+        <v>-0.05594535978273257</v>
       </c>
       <c r="D2" t="n">
-        <v>1.36999909091687e-14</v>
+        <v>0.0657289454088951</v>
       </c>
       <c r="E2" t="n">
-        <v>0.03461451396166826</v>
+        <v>0.02553986469241084</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.3527036992263015</v>
+        <v>-0.1155442666353594</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.2129925928879504</v>
+        <v>0.003653547069894257</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>[-0.352704, -0.212993]</t>
+          <t>[-0.115544, 0.003654]</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>7.534995000042784e-14</v>
+        <v>0.3286447270444754</v>
       </c>
       <c r="J2" t="n">
-        <v>0.3742131474374075</v>
+        <v>0.563913281555328</v>
       </c>
       <c r="K2" t="n">
-        <v>-0.2828481460571259</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>AV_2</t>
+          <t>VA_4</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>-0.2386579046833174</v>
+        <v>0.04249990381134629</v>
       </c>
       <c r="D3" t="n">
-        <v>1.706942952742104e-10</v>
+        <v>0.1327907433926695</v>
       </c>
       <c r="E3" t="n">
-        <v>0.03473829405018308</v>
+        <v>0.033898007581214</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.3104508195280604</v>
+        <v>-0.01296208409305214</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.1668649898385743</v>
+        <v>0.09796189171574471</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>[-0.310451, -0.166865]</t>
+          <t>[-0.012962, 0.097962]</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>4.694093120040785e-10</v>
+        <v>0.4426358113088983</v>
       </c>
       <c r="J3" t="n">
-        <v>0.2806748164326336</v>
+        <v>0.6562658924156471</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.2386579046833174</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>VA_4</t>
+          <t>VLa_5</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-0.1275662382078852</v>
+        <v>0.008312956983324772</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0001978171308036089</v>
+        <v>0.7852221035731102</v>
       </c>
       <c r="E4" t="n">
-        <v>0.04334399563367821</v>
+        <v>0.02757799470435522</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.1943814293479179</v>
+        <v>-0.05159599972900225</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.06075104706785246</v>
+        <v>0.0682219136956518</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>[-0.194381, -0.060751]</t>
+          <t>[-0.051596, 0.068222]</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>0.0001978171308036089</v>
+        <v>0.7852221035731102</v>
       </c>
       <c r="J4" t="n">
-        <v>0.4329151887200363</v>
+        <v>0.5739640018044544</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.1275662382078852</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>VLa_5</t>
+          <t>VLP_6</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>-0.1406086080481011</v>
+        <v>0.02192436261418324</v>
       </c>
       <c r="D5" t="n">
-        <v>4.535561571163648e-05</v>
+        <v>0.2925808412987462</v>
       </c>
       <c r="E5" t="n">
-        <v>0.03481261892170393</v>
+        <v>0.0198852695321954</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.2077146572799533</v>
+        <v>-0.01896460408055503</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.07350255881624901</v>
+        <v>0.06281332930892151</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>[-0.207715, -0.073503]</t>
+          <t>[-0.018965, 0.062813]</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>4.989117728280013e-05</v>
+        <v>0.7314521032468655</v>
       </c>
       <c r="J5" t="n">
-        <v>0.3923521767729949</v>
+        <v>0.8094307412556222</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.1406086080481011</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>VLP_6</t>
+          <t>VPL_7</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>-0.2153659251206056</v>
+        <v>0.008710011278819409</v>
       </c>
       <c r="D6" t="n">
-        <v>3.083482439149176e-09</v>
+        <v>0.7158715648327176</v>
       </c>
       <c r="E6" t="n">
-        <v>0.03515579953464267</v>
+        <v>0.02549730031384117</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.2853804429037499</v>
+        <v>-0.03828590634536476</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.1453514073374612</v>
+        <v>0.05570592890300358</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>[-0.285380, -0.145351]</t>
+          <t>[-0.038286, 0.055706]</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>4.845472404377277e-09</v>
+        <v>0.7852221035731102</v>
       </c>
       <c r="J6" t="n">
-        <v>0.364840792410332</v>
+        <v>0.7466519899099058</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.2153659251206056</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>VPL_7</t>
+          <t>Pul_8</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-0.2288370062485052</v>
+        <v>-0.05888321540775257</v>
       </c>
       <c r="D7" t="n">
-        <v>1.877565138698976e-09</v>
+        <v>0.0001320510407233049</v>
       </c>
       <c r="E7" t="n">
-        <v>0.04037443724028335</v>
+        <v>0.0169263282054592</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.3021895163163656</v>
+        <v>-0.08889823458667337</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.1554844961806447</v>
+        <v>-0.02886819622883178</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>[-0.302190, -0.155484]</t>
+          <t>[-0.088898, -0.028868]</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>3.442202754281457e-09</v>
+        <v>0.001320510407233048</v>
       </c>
       <c r="J7" t="n">
-        <v>0.298394459690187</v>
+        <v>0.8965957710854626</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.2288370062485052</v>
+        <v>-0.05888321540775257</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Pul_8</t>
+          <t>LGN_9</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>-0.3306488496651777</v>
+        <v>-0.019123620445045</v>
       </c>
       <c r="D8" t="n">
-        <v>1.017194030734887e-17</v>
+        <v>0.5452040174580715</v>
       </c>
       <c r="E8" t="n">
-        <v>0.03751828072158667</v>
+        <v>0.03124457284180053</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.4034204192941265</v>
+        <v>-0.08119737092027834</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.257877280036229</v>
+        <v>0.04295013003018835</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>[-0.403420, -0.257877]</t>
+          <t>[-0.081197, 0.042950]</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>1.118913433808376e-16</v>
+        <v>0.7852221035731102</v>
       </c>
       <c r="J8" t="n">
-        <v>0.3090440584709645</v>
+        <v>0.5556787779672687</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.3306488496651777</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>LGN_9</t>
+          <t>MGN_10</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>-0.2389826464316465</v>
+        <v>-0.009271867575499837</v>
       </c>
       <c r="D9" t="n">
-        <v>6.933129953546609e-09</v>
+        <v>0.7212143933194799</v>
       </c>
       <c r="E9" t="n">
-        <v>0.04435413978223735</v>
+        <v>0.02291181769811465</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.3185481830284232</v>
+        <v>-0.0603012838703267</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.1594171098348697</v>
+        <v>0.04175754871932703</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>[-0.318548, -0.159417]</t>
+          <t>[-0.060301, 0.041758]</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>9.533053686126587e-09</v>
+        <v>0.7852221035731102</v>
       </c>
       <c r="J9" t="n">
-        <v>0.1701551606949825</v>
+        <v>0.7024731547744807</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.2389826464316465</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>MGN_10</t>
+          <t>CM_11</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>-0.2225821996937384</v>
+        <v>0.01406906241247959</v>
       </c>
       <c r="D10" t="n">
-        <v>1.693418313133269e-09</v>
+        <v>0.6306878754009462</v>
       </c>
       <c r="E10" t="n">
-        <v>0.03645537421522035</v>
+        <v>0.02509249670934655</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.2937239455883065</v>
+        <v>-0.0434002199385868</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.1514404537991702</v>
+        <v>0.07153834476354597</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>[-0.293724, -0.151440]</t>
+          <t>[-0.043400, 0.071538]</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>3.442202754281457e-09</v>
+        <v>0.7852221035731102</v>
       </c>
       <c r="J10" t="n">
-        <v>0.3426452357463446</v>
+        <v>0.6157516319818271</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.2225821996937384</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>CM_11</t>
+          <t>MD_Pf_12</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>-0.1790321914503122</v>
+        <v>0.007100405750369639</v>
       </c>
       <c r="D11" t="n">
-        <v>1.384574558799017e-06</v>
+        <v>0.6863800055980636</v>
       </c>
       <c r="E11" t="n">
-        <v>0.03309469003506695</v>
+        <v>0.0196224544284776</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.2509593478163804</v>
+        <v>-0.02743466605393511</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.1071050350842441</v>
+        <v>0.04163547755467439</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>[-0.250959, -0.107105]</t>
+          <t>[-0.027435, 0.041635]</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>1.692257794087688e-06</v>
+        <v>0.7852221035731102</v>
       </c>
       <c r="J11" t="n">
-        <v>0.3157857950849888</v>
+        <v>0.8690366717937915</v>
       </c>
       <c r="K11" t="n">
-        <v>-0.1790321914503122</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>MD_Pf_12</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>-0.2690984011824953</v>
-      </c>
-      <c r="D12" t="n">
-        <v>8.795097975091295e-12</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.03051872270009511</v>
-      </c>
-      <c r="F12" t="n">
-        <v>-0.3445966614498267</v>
-      </c>
-      <c r="G12" t="n">
-        <v>-0.1936001409151639</v>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>[-0.344597, -0.193600]</t>
-        </is>
-      </c>
-      <c r="I12" t="n">
-        <v>3.224869257533475e-11</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0.2885101877856169</v>
-      </c>
-      <c r="K12" t="n">
-        <v>-0.2690984011824953</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2932,7 +2737,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2994,431 +2799,392 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>THALAMUS_1</t>
+          <t>AV_2</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.363777831113971</v>
+        <v>0.007383605803901738</v>
       </c>
       <c r="D2" t="n">
-        <v>1.919437419055453e-17</v>
+        <v>0.8385214569629597</v>
       </c>
       <c r="E2" t="n">
-        <v>0.04313739844954225</v>
+        <v>0.03621056343578313</v>
       </c>
       <c r="F2" t="n">
-        <v>0.2829672404752995</v>
+        <v>-0.06377684099901892</v>
       </c>
       <c r="G2" t="n">
-        <v>0.4445884217526425</v>
+        <v>0.0785440526068224</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>[0.282967, 0.444588]</t>
+          <t>[-0.063777, 0.078544]</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>2.111381160960998e-16</v>
+        <v>0.8385214569629597</v>
       </c>
       <c r="J2" t="n">
-        <v>0.3914905348355714</v>
+        <v>0.5607409469297278</v>
       </c>
       <c r="K2" t="n">
-        <v>0.363777831113971</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>AV_2</t>
+          <t>VA_4</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.2499623584641519</v>
+        <v>0.009082117143164151</v>
       </c>
       <c r="D3" t="n">
-        <v>1.386464304026647e-08</v>
+        <v>0.7873955925424732</v>
       </c>
       <c r="E3" t="n">
-        <v>0.04057308747254555</v>
+        <v>0.0347582406758179</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1649558615332549</v>
+        <v>-0.05705584873005709</v>
       </c>
       <c r="G3" t="n">
-        <v>0.3349688553950488</v>
+        <v>0.07522008301638539</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>[0.164956, 0.334969]</t>
+          <t>[-0.057056, 0.075220]</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>1.694567482699236e-08</v>
+        <v>0.8385214569629597</v>
       </c>
       <c r="J3" t="n">
-        <v>0.2672217927589982</v>
+        <v>0.6546332303684339</v>
       </c>
       <c r="K3" t="n">
-        <v>0.2499623584641519</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>VA_4</t>
+          <t>VLa_5</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.219920091198304</v>
+        <v>0.0209468896611776</v>
       </c>
       <c r="D4" t="n">
-        <v>3.424216791273572e-08</v>
+        <v>0.56374079618624</v>
       </c>
       <c r="E4" t="n">
-        <v>0.04005793160183983</v>
+        <v>0.03454153635489471</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1429310828523183</v>
+        <v>-0.05030499098978222</v>
       </c>
       <c r="G4" t="n">
-        <v>0.2969090995442897</v>
+        <v>0.09219877031213741</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>[0.142931, 0.296909]</t>
+          <t>[-0.050305, 0.092199]</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>3.766638470400929e-08</v>
+        <v>0.8385214569629597</v>
       </c>
       <c r="J4" t="n">
-        <v>0.452906884148458</v>
+        <v>0.5742030328468152</v>
       </c>
       <c r="K4" t="n">
-        <v>0.219920091198304</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>VLa_5</t>
+          <t>VLP_6</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.2081639455449239</v>
+        <v>-0.008176503345716702</v>
       </c>
       <c r="D5" t="n">
-        <v>2.281315389048555e-07</v>
+        <v>0.7415848972207475</v>
       </c>
       <c r="E5" t="n">
-        <v>0.03922901552405331</v>
+        <v>0.02604986284197009</v>
       </c>
       <c r="F5" t="n">
-        <v>0.130298443847835</v>
+        <v>-0.05687354926053842</v>
       </c>
       <c r="G5" t="n">
-        <v>0.2860294472420128</v>
+        <v>0.04052054256910502</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>[0.130298, 0.286029]</t>
+          <t>[-0.056874, 0.040521]</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>2.281315389048555e-07</v>
+        <v>0.8385214569629597</v>
       </c>
       <c r="J5" t="n">
-        <v>0.4055367794595286</v>
+        <v>0.8090177861097805</v>
       </c>
       <c r="K5" t="n">
-        <v>0.2081639455449239</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>VLP_6</t>
+          <t>VPL_7</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.2947985193935562</v>
+        <v>0.0350914471011553</v>
       </c>
       <c r="D6" t="n">
-        <v>3.27762921596554e-12</v>
+        <v>0.2173644130577758</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0423122384878856</v>
+        <v>0.03079580264566631</v>
       </c>
       <c r="F6" t="n">
-        <v>0.213842171542482</v>
+        <v>-0.02073409140098124</v>
       </c>
       <c r="G6" t="n">
-        <v>0.3757548672446304</v>
+        <v>0.09091698560329184</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>[0.213842, 0.375755]</t>
+          <t>[-0.020734, 0.090917]</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>7.210784275124189e-12</v>
+        <v>0.8385214569629597</v>
       </c>
       <c r="J6" t="n">
-        <v>0.382958430166906</v>
+        <v>0.7474134689022506</v>
       </c>
       <c r="K6" t="n">
-        <v>0.2947985193935562</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>VPL_7</t>
+          <t>Pul_8</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.3341854066582388</v>
+        <v>0.004686313516578885</v>
       </c>
       <c r="D7" t="n">
-        <v>3.924290196223039e-14</v>
+        <v>0.7997102555009488</v>
       </c>
       <c r="E7" t="n">
-        <v>0.04674145093172746</v>
+        <v>0.01797811709906252</v>
       </c>
       <c r="F7" t="n">
-        <v>0.250074750470937</v>
+        <v>-0.03158891827133881</v>
       </c>
       <c r="G7" t="n">
-        <v>0.4182960628455406</v>
+        <v>0.04096154530449657</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>[0.250075, 0.418296]</t>
+          <t>[-0.031589, 0.040962]</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>1.438906405281781e-13</v>
+        <v>0.8385214569629597</v>
       </c>
       <c r="J7" t="n">
-        <v>0.3296967791643436</v>
+        <v>0.8932842406378811</v>
       </c>
       <c r="K7" t="n">
-        <v>0.3341854066582388</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Pul_8</t>
+          <t>LGN_9</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.3626428788411847</v>
+        <v>0.01521656230296636</v>
       </c>
       <c r="D8" t="n">
-        <v>1.559739770598081e-15</v>
+        <v>0.6857887777408416</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0460647994373795</v>
+        <v>0.04257008189749497</v>
       </c>
       <c r="F8" t="n">
-        <v>0.2763513876656371</v>
+        <v>-0.0586468919168499</v>
       </c>
       <c r="G8" t="n">
-        <v>0.4489343700167324</v>
+        <v>0.08908001652278262</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>[0.276351, 0.448934]</t>
+          <t>[-0.058647, 0.089080]</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>8.578568738289445e-15</v>
+        <v>0.8385214569629597</v>
       </c>
       <c r="J8" t="n">
-        <v>0.2940579818347346</v>
+        <v>0.5554839684472559</v>
       </c>
       <c r="K8" t="n">
-        <v>0.3626428788411847</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>LGN_9</t>
+          <t>MGN_10</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.2987411683752589</v>
+        <v>0.02226916156133042</v>
       </c>
       <c r="D9" t="n">
-        <v>6.094208109756722e-10</v>
+        <v>0.4711790189927436</v>
       </c>
       <c r="E9" t="n">
-        <v>0.04930082041763328</v>
+        <v>0.02908934896381998</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2058771217624582</v>
+        <v>-0.03841322521688873</v>
       </c>
       <c r="G9" t="n">
-        <v>0.3916052149880596</v>
+        <v>0.08295154833954957</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>[0.205877, 0.391605]</t>
+          <t>[-0.038413, 0.082952]</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>8.379536150915493e-10</v>
+        <v>0.8385214569629597</v>
       </c>
       <c r="J9" t="n">
-        <v>0.1786120492981538</v>
+        <v>0.7027256889349982</v>
       </c>
       <c r="K9" t="n">
-        <v>0.2987411683752589</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>MGN_10</t>
+          <t>CM_11</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.2948275233966268</v>
+        <v>0.03159286379034325</v>
       </c>
       <c r="D10" t="n">
-        <v>7.881637493656552e-12</v>
+        <v>0.364012598901409</v>
       </c>
       <c r="E10" t="n">
-        <v>0.04309757115736179</v>
+        <v>0.0327454853158049</v>
       </c>
       <c r="F10" t="n">
-        <v>0.2123105907076505</v>
+        <v>-0.03673270475200406</v>
       </c>
       <c r="G10" t="n">
-        <v>0.3773444560856031</v>
+        <v>0.09991843233269056</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>[0.212311, 0.377344]</t>
+          <t>[-0.036733, 0.099918]</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>1.444966873837034e-11</v>
+        <v>0.8385214569629597</v>
       </c>
       <c r="J10" t="n">
-        <v>0.3573964175539167</v>
+        <v>0.6162449452752623</v>
       </c>
       <c r="K10" t="n">
-        <v>0.2948275233966268</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>CM_11</t>
+          <t>MD_Pf_12</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.2732007810524334</v>
+        <v>-0.03150297527664891</v>
       </c>
       <c r="D11" t="n">
-        <v>2.359337531111705e-10</v>
+        <v>0.1316668900046285</v>
       </c>
       <c r="E11" t="n">
-        <v>0.04076356334923593</v>
+        <v>0.02109652083621447</v>
       </c>
       <c r="F11" t="n">
-        <v>0.1903431516823693</v>
+        <v>-0.07249450595142413</v>
       </c>
       <c r="G11" t="n">
-        <v>0.3560584104224975</v>
+        <v>0.009488555398126305</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>[0.190343, 0.356058]</t>
+          <t>[-0.072495, 0.009489]</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>3.707530406032679e-10</v>
+        <v>0.8385214569629597</v>
       </c>
       <c r="J11" t="n">
-        <v>0.3402528463204869</v>
+        <v>0.8696339926138884</v>
       </c>
       <c r="K11" t="n">
-        <v>0.2732007810524334</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>MD_Pf_12</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>0.3271791460534005</v>
-      </c>
-      <c r="D12" t="n">
-        <v>1.369450909211227e-12</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.04819774148700044</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.2389582295235205</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0.4154000625832804</v>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>[0.238958, 0.415400]</t>
-        </is>
-      </c>
-      <c r="I12" t="n">
-        <v>3.765990000330874e-12</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0.2940984399163286</v>
-      </c>
-      <c r="K12" t="n">
-        <v>0.3271791460534005</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3432,7 +3198,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3494,431 +3260,392 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>THALAMUS_1</t>
+          <t>AV_2</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.2012039722164457</v>
+        <v>0.02086740132967175</v>
       </c>
       <c r="D2" t="n">
-        <v>9.929843051582725e-07</v>
+        <v>0.5168622521127125</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0413453229261907</v>
+        <v>0.03355484634080833</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1214842136352777</v>
+        <v>-0.04234753447083354</v>
       </c>
       <c r="G2" t="n">
-        <v>0.2809237307976137</v>
+        <v>0.08408233713017703</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>[0.121484, 0.280924]</t>
+          <t>[-0.042348, 0.084082]</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>5.461413678370499e-06</v>
+        <v>0.7383746458753037</v>
       </c>
       <c r="J2" t="n">
-        <v>0.3245303408810305</v>
+        <v>0.5611011736422956</v>
       </c>
       <c r="K2" t="n">
-        <v>0.2012039722164457</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>AV_2</t>
+          <t>VA_4</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.1545743858326961</v>
+        <v>0.0397935729435373</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0002062944892679597</v>
+        <v>0.1832297661733801</v>
       </c>
       <c r="E3" t="n">
-        <v>0.03860382935666595</v>
+        <v>0.02891820359306169</v>
       </c>
       <c r="F3" t="n">
-        <v>0.07337830363125325</v>
+        <v>-0.01887571743000369</v>
       </c>
       <c r="G3" t="n">
-        <v>0.235770468034139</v>
+        <v>0.09846286331707829</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>[0.073378, 0.235770]</t>
+          <t>[-0.018876, 0.098463]</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>0.0002836549227434445</v>
+        <v>0.4731894831410917</v>
       </c>
       <c r="J3" t="n">
-        <v>0.2374267345727278</v>
+        <v>0.6559019747340076</v>
       </c>
       <c r="K3" t="n">
-        <v>0.1545743858326961</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>VA_4</t>
+          <t>VLa_5</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.1551258935022795</v>
+        <v>0.03621617276420892</v>
       </c>
       <c r="D4" t="n">
-        <v>3.670170061004754e-05</v>
+        <v>0.2611521910227292</v>
       </c>
       <c r="E4" t="n">
-        <v>0.03667917783722956</v>
+        <v>0.030481167304513</v>
       </c>
       <c r="F4" t="n">
-        <v>0.08198570275269913</v>
+        <v>-0.02704223057270198</v>
       </c>
       <c r="G4" t="n">
-        <v>0.22826608425186</v>
+        <v>0.09947457610111983</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>[0.081986, 0.228266]</t>
+          <t>[-0.027042, 0.099475]</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>6.72864511184205e-05</v>
+        <v>0.5223043820454584</v>
       </c>
       <c r="J4" t="n">
-        <v>0.4368046034823376</v>
+        <v>0.5750596406980454</v>
       </c>
       <c r="K4" t="n">
-        <v>0.1551258935022795</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>VLa_5</t>
+          <t>VLP_6</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.1396131158406421</v>
+        <v>-0.004757003475837776</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0002328064263543275</v>
+        <v>0.8290923834606134</v>
       </c>
       <c r="E5" t="n">
-        <v>0.03639159429074737</v>
+        <v>0.0223365774431611</v>
       </c>
       <c r="F5" t="n">
-        <v>0.06565490000516976</v>
+        <v>-0.04803738105824171</v>
       </c>
       <c r="G5" t="n">
-        <v>0.2135713316761144</v>
+        <v>0.03852337410656616</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>[0.065655, 0.213571]</t>
+          <t>[-0.048037, 0.038523]</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>0.0002845411877664003</v>
+        <v>0.9553649949293395</v>
       </c>
       <c r="J5" t="n">
-        <v>0.3882826625442015</v>
+        <v>0.8089920688351669</v>
       </c>
       <c r="K5" t="n">
-        <v>0.1396131158406421</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>VLP_6</t>
+          <t>VPL_7</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.1624033360091812</v>
+        <v>0.04384036823819739</v>
       </c>
       <c r="D6" t="n">
-        <v>5.626035356143589e-05</v>
+        <v>0.08265077368885285</v>
       </c>
       <c r="E6" t="n">
-        <v>0.04162841602987712</v>
+        <v>0.02503901727507608</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0839087353055511</v>
+        <v>-0.005692204169292635</v>
       </c>
       <c r="G6" t="n">
-        <v>0.2408979367128114</v>
+        <v>0.09337294064568741</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>[0.083909, 0.240898]</t>
+          <t>[-0.005692, 0.093373]</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>8.840912702511353e-05</v>
+        <v>0.4132538684442643</v>
       </c>
       <c r="J6" t="n">
-        <v>0.3383393651501678</v>
+        <v>0.748227819462542</v>
       </c>
       <c r="K6" t="n">
-        <v>0.1624033360091812</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>VPL_7</t>
+          <t>Pul_8</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.2098624044310598</v>
+        <v>0.0007280521044546392</v>
       </c>
       <c r="D7" t="n">
-        <v>6.162060830793335e-07</v>
+        <v>0.9646236312385743</v>
       </c>
       <c r="E7" t="n">
-        <v>0.04200767615489188</v>
+        <v>0.01617533327176772</v>
       </c>
       <c r="F7" t="n">
-        <v>0.128304587334982</v>
+        <v>-0.03151222353902126</v>
       </c>
       <c r="G7" t="n">
-        <v>0.2914202215271376</v>
+        <v>0.03296832774793054</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>[0.128305, 0.291420]</t>
+          <t>[-0.031512, 0.032968]</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>5.461413678370499e-06</v>
+        <v>0.9646236312385743</v>
       </c>
       <c r="J7" t="n">
-        <v>0.2811412372563813</v>
+        <v>0.8932698086974048</v>
       </c>
       <c r="K7" t="n">
-        <v>0.2098624044310598</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Pul_8</t>
+          <t>LGN_9</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.1990503231763727</v>
+        <v>0.005903076310192691</v>
       </c>
       <c r="D8" t="n">
-        <v>4.915754385379004e-06</v>
+        <v>0.8598284954364055</v>
       </c>
       <c r="E8" t="n">
-        <v>0.04417884367982516</v>
+        <v>0.03435803189441664</v>
       </c>
       <c r="F8" t="n">
-        <v>0.1144373520365284</v>
+        <v>-0.05974940465931686</v>
       </c>
       <c r="G8" t="n">
-        <v>0.283663294316217</v>
+        <v>0.07155555727970225</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>[0.114437, 0.283663]</t>
+          <t>[-0.059749, 0.071556]</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>1.802443274638968e-05</v>
+        <v>0.9553649949293395</v>
       </c>
       <c r="J8" t="n">
-        <v>0.2258054755389928</v>
+        <v>0.5553563290254007</v>
       </c>
       <c r="K8" t="n">
-        <v>0.1990503231763727</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>LGN_9</t>
+          <t>MGN_10</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.1636383358234076</v>
+        <v>0.02063445354251997</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0003558590832247577</v>
+        <v>0.4524736378283877</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0439499741613503</v>
+        <v>0.02804551263089654</v>
       </c>
       <c r="F9" t="n">
-        <v>0.07425279856635494</v>
+        <v>-0.03329183786477079</v>
       </c>
       <c r="G9" t="n">
-        <v>0.2530238730804604</v>
+        <v>0.07456074494981073</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>[0.074253, 0.253024]</t>
+          <t>[-0.033292, 0.074561]</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>0.0003914449915472335</v>
+        <v>0.7383746458753037</v>
       </c>
       <c r="J9" t="n">
-        <v>0.1319779669455398</v>
+        <v>0.7027548276292692</v>
       </c>
       <c r="K9" t="n">
-        <v>0.1636383358234076</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>MGN_10</t>
+          <t>CM_11</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.1721251214753012</v>
+        <v>0.04058318083271145</v>
       </c>
       <c r="D10" t="n">
-        <v>2.677055598111944e-05</v>
+        <v>0.1892757932564367</v>
       </c>
       <c r="E10" t="n">
-        <v>0.04171884367343285</v>
+        <v>0.02924474374897561</v>
       </c>
       <c r="F10" t="n">
-        <v>0.09238765280079432</v>
+        <v>-0.02007918222231457</v>
       </c>
       <c r="G10" t="n">
-        <v>0.2518625901498082</v>
+        <v>0.1012455438877375</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>[0.092388, 0.251863]</t>
+          <t>[-0.020079, 0.101246]</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>5.889522315846278e-05</v>
+        <v>0.4731894831410917</v>
       </c>
       <c r="J10" t="n">
-        <v>0.3155763628950334</v>
+        <v>0.6169919720263382</v>
       </c>
       <c r="K10" t="n">
-        <v>0.1721251214753012</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>CM_11</t>
+          <t>MD_Pf_12</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.1746944841993937</v>
+        <v>-0.05645515780868141</v>
       </c>
       <c r="D11" t="n">
-        <v>1.897489809804462e-05</v>
+        <v>0.002276620555517609</v>
       </c>
       <c r="E11" t="n">
-        <v>0.03976623270364581</v>
+        <v>0.0182194669622464</v>
       </c>
       <c r="F11" t="n">
-        <v>0.09525771094347334</v>
+        <v>-0.09260789632063054</v>
       </c>
       <c r="G11" t="n">
-        <v>0.2541312574553141</v>
+        <v>-0.02030241929673227</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>[0.095258, 0.254131]</t>
+          <t>[-0.092608, -0.020302]</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>5.218096976962272e-05</v>
+        <v>0.02276620555517609</v>
       </c>
       <c r="J11" t="n">
-        <v>0.3083301774429285</v>
+        <v>0.8716073620023811</v>
       </c>
       <c r="K11" t="n">
-        <v>0.1746944841993937</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>MD_Pf_12</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>0.1422593134089052</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0.001274435828278927</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.04552929703856541</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.05601933142894387</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0.2284992953888665</v>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>[0.056019, 0.228499]</t>
-        </is>
-      </c>
-      <c r="I12" t="n">
-        <v>0.001274435828278927</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0.2305835882053499</v>
-      </c>
-      <c r="K12" t="n">
-        <v>0.1422593134089052</v>
+        <v>-0.05645515780868141</v>
       </c>
     </row>
   </sheetData>
@@ -3932,7 +3659,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3994,431 +3721,392 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>THALAMUS_1</t>
+          <t>AV_2</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.4250873027162566</v>
+        <v>-0.009027833543027153</v>
       </c>
       <c r="D2" t="n">
-        <v>1.889738712366386e-21</v>
+        <v>0.8167361072535648</v>
       </c>
       <c r="E2" t="n">
-        <v>0.04739540927278216</v>
+        <v>0.03739392264785205</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3415599637542226</v>
+        <v>-0.08553690179958734</v>
       </c>
       <c r="G2" t="n">
-        <v>0.5086146416782906</v>
+        <v>0.06748123471353304</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>[0.341560, 0.508615]</t>
+          <t>[-0.085537, 0.067481]</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>2.078712583603025e-20</v>
+        <v>0.9389243699156311</v>
       </c>
       <c r="J2" t="n">
-        <v>0.4150109645216811</v>
+        <v>0.5607525372798263</v>
       </c>
       <c r="K2" t="n">
-        <v>0.4250873027162566</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>AV_2</t>
+          <t>VA_4</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.2772852037922503</v>
+        <v>-0.02589970156129635</v>
       </c>
       <c r="D3" t="n">
-        <v>2.187689078588034e-09</v>
+        <v>0.4743074279387159</v>
       </c>
       <c r="E3" t="n">
-        <v>0.04323543508472771</v>
+        <v>0.03781727456212466</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1880193195789653</v>
+        <v>-0.09697589510472139</v>
       </c>
       <c r="G3" t="n">
-        <v>0.3665510880055353</v>
+        <v>0.04517649198212868</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>[0.188019, 0.366551]</t>
+          <t>[-0.096976, 0.045176]</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>2.673842207163154e-09</v>
+        <v>0.9389243699156311</v>
       </c>
       <c r="J3" t="n">
-        <v>0.272891892771447</v>
+        <v>0.6549617435662847</v>
       </c>
       <c r="K3" t="n">
-        <v>0.2772852037922503</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>VA_4</t>
+          <t>VLa_5</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.2266072346733524</v>
+        <v>-0.001539056305834889</v>
       </c>
       <c r="D4" t="n">
-        <v>7.058236283197997e-08</v>
+        <v>0.9685368991774286</v>
       </c>
       <c r="E4" t="n">
-        <v>0.04344764574690056</v>
+        <v>0.03840787357464424</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1453228259486552</v>
+        <v>-0.07817497840800805</v>
       </c>
       <c r="G4" t="n">
-        <v>0.3078916433980495</v>
+        <v>0.07509686579633826</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>[0.145323, 0.307892]</t>
+          <t>[-0.078175, 0.075097]</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>7.764059911517798e-08</v>
+        <v>0.9685368991774286</v>
       </c>
       <c r="J4" t="n">
-        <v>0.4512456712216902</v>
+        <v>0.5738968726237003</v>
       </c>
       <c r="K4" t="n">
-        <v>0.2266072346733524</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>VLa_5</t>
+          <t>VLP_6</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.2210430004670931</v>
+        <v>-0.009223409667805549</v>
       </c>
       <c r="D5" t="n">
-        <v>1.851828658026236e-07</v>
+        <v>0.7293653991827718</v>
       </c>
       <c r="E5" t="n">
-        <v>0.04286866267549058</v>
+        <v>0.02843551000069295</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1389934940550085</v>
+        <v>-0.0615807332231104</v>
       </c>
       <c r="G5" t="n">
-        <v>0.3030925068791777</v>
+        <v>0.04313391388749931</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>[0.138993, 0.303093]</t>
+          <t>[-0.061581, 0.043134]</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>1.851828658026236e-07</v>
+        <v>0.9389243699156311</v>
       </c>
       <c r="J5" t="n">
-        <v>0.4060547383836591</v>
+        <v>0.809022320208133</v>
       </c>
       <c r="K5" t="n">
-        <v>0.2210430004670931</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>VLP_6</t>
+          <t>VPL_7</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.3450707451395961</v>
+        <v>0.0150501680414078</v>
       </c>
       <c r="D6" t="n">
-        <v>7.050510298168974e-15</v>
+        <v>0.6229142679422035</v>
       </c>
       <c r="E6" t="n">
-        <v>0.04644154086543869</v>
+        <v>0.03354016985213051</v>
       </c>
       <c r="F6" t="n">
-        <v>0.2608333854024384</v>
+        <v>-0.04505545717380713</v>
       </c>
       <c r="G6" t="n">
-        <v>0.4293081048767539</v>
+        <v>0.07515579325662272</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>[0.260833, 0.429308]</t>
+          <t>[-0.045055, 0.075156]</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>1.551112265597175e-14</v>
+        <v>0.9389243699156311</v>
       </c>
       <c r="J6" t="n">
-        <v>0.3988515123617496</v>
+        <v>0.7467119902784461</v>
       </c>
       <c r="K6" t="n">
-        <v>0.3450707451395961</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>VPL_7</t>
+          <t>Pul_8</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.367807055486488</v>
+        <v>0.007379416320757948</v>
       </c>
       <c r="D7" t="n">
-        <v>2.383730387830442e-15</v>
+        <v>0.7101839082965701</v>
       </c>
       <c r="E7" t="n">
-        <v>0.05181839713839255</v>
+        <v>0.02051892291994274</v>
       </c>
       <c r="F7" t="n">
-        <v>0.2796650683801278</v>
+        <v>-0.03161976464334289</v>
       </c>
       <c r="G7" t="n">
-        <v>0.4559490425928481</v>
+        <v>0.04637859728485878</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>[0.279665, 0.455949]</t>
+          <t>[-0.031620, 0.046379]</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>6.555258566533715e-15</v>
+        <v>0.9389243699156311</v>
       </c>
       <c r="J7" t="n">
-        <v>0.3376392381123557</v>
+        <v>0.8933012856738027</v>
       </c>
       <c r="K7" t="n">
-        <v>0.367807055486488</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Pul_8</t>
+          <t>LGN_9</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.4251451932038744</v>
+        <v>0.02025437860467486</v>
       </c>
       <c r="D8" t="n">
-        <v>3.799206999186705e-19</v>
+        <v>0.6164474903967925</v>
       </c>
       <c r="E8" t="n">
-        <v>0.04887753544055451</v>
+        <v>0.04593036824261969</v>
       </c>
       <c r="F8" t="n">
-        <v>0.3357774618172147</v>
+        <v>-0.05915440721588471</v>
       </c>
       <c r="G8" t="n">
-        <v>0.5145129245905341</v>
+        <v>0.09966316442523443</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>[0.335777, 0.514513]</t>
+          <t>[-0.059154, 0.099663]</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>2.089563849552688e-18</v>
+        <v>0.9389243699156311</v>
       </c>
       <c r="J8" t="n">
-        <v>0.3186751804600282</v>
+        <v>0.5555679610579647</v>
       </c>
       <c r="K8" t="n">
-        <v>0.4251451932038744</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>LGN_9</t>
+          <t>MGN_10</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.3505356610790545</v>
+        <v>0.01707819143653588</v>
       </c>
       <c r="D9" t="n">
-        <v>4.422464396272932e-12</v>
+        <v>0.6073295443792185</v>
       </c>
       <c r="E9" t="n">
-        <v>0.05416941758093831</v>
+        <v>0.03053526222475915</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2536535930532411</v>
+        <v>-0.04818415354426799</v>
       </c>
       <c r="G9" t="n">
-        <v>0.447417729104868</v>
+        <v>0.08234053641733974</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>[0.253654, 0.447418]</t>
+          <t>[-0.048184, 0.082341]</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>6.949586908428893e-12</v>
+        <v>0.9389243699156311</v>
       </c>
       <c r="J9" t="n">
-        <v>0.1955490316646061</v>
+        <v>0.7025613036441347</v>
       </c>
       <c r="K9" t="n">
-        <v>0.3505356610790545</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>MGN_10</t>
+          <t>CM_11</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.3363007604208247</v>
+        <v>0.01238326374137735</v>
       </c>
       <c r="D10" t="n">
-        <v>1.043728952619688e-13</v>
+        <v>0.7407974420780021</v>
       </c>
       <c r="E10" t="n">
-        <v>0.04636619291830126</v>
+        <v>0.03444152848595437</v>
       </c>
       <c r="F10" t="n">
-        <v>0.2501065347735035</v>
+        <v>-0.06113571336015473</v>
       </c>
       <c r="G10" t="n">
-        <v>0.422494986068146</v>
+        <v>0.08590224084290944</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>[0.250107, 0.422495]</t>
+          <t>[-0.061136, 0.085902]</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>1.913503079802761e-13</v>
+        <v>0.9389243699156311</v>
       </c>
       <c r="J10" t="n">
-        <v>0.3690818898441764</v>
+        <v>0.615650288592839</v>
       </c>
       <c r="K10" t="n">
-        <v>0.3363007604208247</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>CM_11</t>
+          <t>MD_Pf_12</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.297848358229329</v>
+        <v>0.004396860559108885</v>
       </c>
       <c r="D11" t="n">
-        <v>5.286147415125213e-11</v>
+        <v>0.845031932924068</v>
       </c>
       <c r="E11" t="n">
-        <v>0.04451433955144356</v>
+        <v>0.0232677471521749</v>
       </c>
       <c r="F11" t="n">
-        <v>0.2107761343349083</v>
+        <v>-0.0397831195232027</v>
       </c>
       <c r="G11" t="n">
-        <v>0.3849205821237497</v>
+        <v>0.04857684064142047</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>[0.210776, 0.384921]</t>
+          <t>[-0.039783, 0.048577]</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>7.268452695797167e-11</v>
+        <v>0.9389243699156311</v>
       </c>
       <c r="J11" t="n">
-        <v>0.3444113133715884</v>
+        <v>0.8690012438768593</v>
       </c>
       <c r="K11" t="n">
-        <v>0.297848358229329</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>MD_Pf_12</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>0.417426289599158</v>
-      </c>
-      <c r="D12" t="n">
-        <v>3.537802882784993e-18</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.05231565581978086</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.3269371977054421</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0.5079153814928739</v>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>[0.326937, 0.507915]</t>
-        </is>
-      </c>
-      <c r="I12" t="n">
-        <v>1.297194390354497e-17</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0.3317282085700178</v>
-      </c>
-      <c r="K12" t="n">
-        <v>0.417426289599158</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>